<commit_message>
sprint 20: Programm fertig
</commit_message>
<xml_diff>
--- a/documentation/Checklist.xlsx
+++ b/documentation/Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\Software Enginieering 1 Labor\MTCG\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5134427-E0F1-41C1-B36C-71FAF10ECC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72A4B62-5854-428D-A817-E002B152F9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1476" yWindow="-15912" windowWidth="23040" windowHeight="12072" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
+    <workbookView xWindow="0" yWindow="-17388" windowWidth="30936" windowHeight="16776" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -610,7 +610,7 @@
   <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -976,21 +976,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100495F7CC252815B47896F98900E10984C" ma:contentTypeVersion="2" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="afe1b3b164495dc81fdbcdcad6ec8b68">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="207955a2-a3fc-4582-b2ea-e4c7d1fb6048" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b6a42bf87c3f8727d31c248fc1697f6" ns2:_="">
     <xsd:import namespace="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
@@ -1122,10 +1107,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0824ED0-660A-437B-A039-7835C5DD208D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1147,19 +1157,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0824ED0-660A-437B-A039-7835C5DD208D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>